<commit_message>
Update booking at tee time
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/flow_definition.xlsx
+++ b/src/main/resources/input_excel_file/flow_definition.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="11460"/>
   </bookViews>
   <sheets>
-    <sheet name="flow" sheetId="1" r:id="rId1"/>
+    <sheet name="flow_1_player" sheetId="1" r:id="rId1"/>
+    <sheet name="flow_4_player" sheetId="2" r:id="rId2"/>
+    <sheet name="VC_1_player" sheetId="3" r:id="rId3"/>
+    <sheet name="booking_at_tee_time" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="48">
   <si>
     <t>flow_id</t>
   </si>
@@ -50,6 +53,9 @@
     <t>get_booking_price_case_id</t>
   </si>
   <si>
+    <t>edit_booking_at_tee_time_id</t>
+  </si>
+  <si>
     <t>FLOW_001</t>
   </si>
   <si>
@@ -71,6 +77,9 @@
     <t>BP_001</t>
   </si>
   <si>
+    <t>ED_TT_001</t>
+  </si>
+  <si>
     <t>FLOW_002</t>
   </si>
   <si>
@@ -83,6 +92,9 @@
     <t>BB_002</t>
   </si>
   <si>
+    <t>ED_TT_002</t>
+  </si>
+  <si>
     <t>FLOW_003</t>
   </si>
   <si>
@@ -92,6 +104,9 @@
     <t>BB_003</t>
   </si>
   <si>
+    <t>ED_TT_003</t>
+  </si>
+  <si>
     <t>FLOW_004</t>
   </si>
   <si>
@@ -104,6 +119,9 @@
     <t>BB_004</t>
   </si>
   <si>
+    <t>ED_TT_004</t>
+  </si>
+  <si>
     <t>FLOW_005</t>
   </si>
   <si>
@@ -114,6 +132,48 @@
   </si>
   <si>
     <t>BB_005</t>
+  </si>
+  <si>
+    <t>ED_TT_005</t>
+  </si>
+  <si>
+    <t>create_booking_4_player_case_id</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_001</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_002</t>
+  </si>
+  <si>
+    <t>QF_003</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_003</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_004</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_005</t>
+  </si>
+  <si>
+    <t>create_booking_Voucher_case_id</t>
+  </si>
+  <si>
+    <t>BB_VC_VST_001</t>
+  </si>
+  <si>
+    <t>BB_VC_VST_002</t>
+  </si>
+  <si>
+    <t>BB_VC_VST_003</t>
+  </si>
+  <si>
+    <t>BB_VC_VST_004</t>
+  </si>
+  <si>
+    <t>BB_VC_VST_005</t>
   </si>
 </sst>
 </file>
@@ -126,14 +186,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,172 +688,175 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1122,10 +1178,539 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.1428571428571" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.2857142857143" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="30" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:8">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.8571428571429" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.2857142857143" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="30" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:8">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5714285714286" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.2857142857143" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:7">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="30" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
@@ -1165,119 +1750,119 @@
     </row>
     <row r="2" s="1" customFormat="1" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" ht="30" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update method cho api edit booking at tee time
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/flow_definition.xlsx
+++ b/src/main/resources/input_excel_file/flow_definition.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11460"/>
+    <workbookView windowWidth="30240" windowHeight="13080" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="flow_1_player" sheetId="1" r:id="rId1"/>
     <sheet name="flow_4_player" sheetId="2" r:id="rId2"/>
     <sheet name="VC_1_player" sheetId="3" r:id="rId3"/>
     <sheet name="booking_at_tee_time" sheetId="4" r:id="rId4"/>
+    <sheet name="Test" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="49">
   <si>
     <t>flow_id</t>
   </si>
@@ -174,6 +175,9 @@
   </si>
   <si>
     <t>BB_VC_VST_005</t>
+  </si>
+  <si>
+    <t>Booking khách lẻ sửa booking tại tee time</t>
   </si>
 </sst>
 </file>
@@ -181,10 +185,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -691,16 +695,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -833,7 +837,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -854,9 +858,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -867,7 +868,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1180,21 +1181,21 @@
   <sheetPr/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.1428571428571" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.2857142857143" style="1"/>
+    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.2890625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:8">
@@ -1223,7 +1224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:8">
+    <row r="2" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1245,11 +1246,11 @@
       <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:8">
+    <row r="3" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1271,11 +1272,11 @@
       <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="30" spans="1:8">
+    <row r="4" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1295,11 +1296,11 @@
       <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:8">
+    <row r="5" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1321,11 +1322,11 @@
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:8">
+    <row r="6" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -1347,7 +1348,7 @@
       <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1366,17 +1367,17 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.8571428571429" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.2857142857143" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.2857142857143" style="1"/>
+    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.859375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.2890625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.2890625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:8">
@@ -1405,7 +1406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:8">
+    <row r="2" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1427,11 +1428,11 @@
       <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:8">
+    <row r="3" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1453,11 +1454,11 @@
       <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="30" spans="1:8">
+    <row r="4" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1479,11 +1480,11 @@
       <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:8">
+    <row r="5" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1505,11 +1506,11 @@
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:8">
+    <row r="6" s="1" customFormat="1" ht="17" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -1531,7 +1532,7 @@
       <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1550,16 +1551,16 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5714285714286" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.2857142857143" style="1"/>
+    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.2890625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:7">
@@ -1585,7 +1586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:7">
+    <row r="2" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1598,7 +1599,7 @@
       <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="6" t="s">
         <v>43</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -1608,7 +1609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:7">
+    <row r="3" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1621,7 +1622,7 @@
       <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1631,7 +1632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="30" spans="1:7">
+    <row r="4" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1642,7 +1643,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>45</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1652,7 +1653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:7">
+    <row r="5" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1665,7 +1666,7 @@
       <c r="D5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>46</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1675,7 +1676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:7">
+    <row r="6" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -1688,7 +1689,7 @@
       <c r="D6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1713,16 +1714,16 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.2857142857143" style="1"/>
+    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.2890625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:7">
@@ -1748,7 +1749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:7">
+    <row r="2" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1771,7 +1772,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:7">
+    <row r="3" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1794,7 +1795,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="30" spans="1:7">
+    <row r="4" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1815,7 +1816,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:7">
+    <row r="5" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1838,7 +1839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:7">
+    <row r="6" s="1" customFormat="1" ht="17" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -1859,6 +1860,86 @@
       </c>
       <c r="G6" s="5" t="s">
         <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.2890625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="34" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create test script edit booking 1 player
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/flow_definition.xlsx
+++ b/src/main/resources/input_excel_file/flow_definition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13080" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="flow_1_player" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="52">
   <si>
     <t>flow_id</t>
   </si>
@@ -102,6 +102,9 @@
     <t>Kiểm tra flow booking member guest</t>
   </si>
   <si>
+    <t>QF_003</t>
+  </si>
+  <si>
     <t>BB_003</t>
   </si>
   <si>
@@ -135,30 +138,30 @@
     <t>BB_005</t>
   </si>
   <si>
+    <t>ED_TT_006</t>
+  </si>
+  <si>
+    <t>create_booking_4_player_case_id</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_001</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_002</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_003</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_004</t>
+  </si>
+  <si>
+    <t>BB_4_PLAYER_005</t>
+  </si>
+  <si>
     <t>ED_TT_005</t>
   </si>
   <si>
-    <t>create_booking_4_player_case_id</t>
-  </si>
-  <si>
-    <t>BB_4_PLAYER_001</t>
-  </si>
-  <si>
-    <t>BB_4_PLAYER_002</t>
-  </si>
-  <si>
-    <t>QF_003</t>
-  </si>
-  <si>
-    <t>BB_4_PLAYER_003</t>
-  </si>
-  <si>
-    <t>BB_4_PLAYER_004</t>
-  </si>
-  <si>
-    <t>BB_4_PLAYER_005</t>
-  </si>
-  <si>
     <t>create_booking_Voucher_case_id</t>
   </si>
   <si>
@@ -177,7 +180,13 @@
     <t>BB_VC_VST_005</t>
   </si>
   <si>
-    <t>Booking khách lẻ sửa booking tại tee time</t>
+    <t>edit_booking_1_player_id</t>
+  </si>
+  <si>
+    <t>EB_001</t>
+  </si>
+  <si>
+    <t>EB_002</t>
   </si>
 </sst>
 </file>
@@ -185,10 +194,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -695,16 +704,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -837,7 +846,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -854,10 +863,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -868,7 +880,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1182,20 +1194,20 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.2890625" style="1"/>
+    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.1428571428571" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.2857142857143" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:8">
@@ -1224,7 +1236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="17" spans="1:8">
+    <row r="2" s="1" customFormat="1" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1237,7 +1249,7 @@
       <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -1246,11 +1258,11 @@
       <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="17" spans="1:8">
+    <row r="3" s="1" customFormat="1" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1263,7 +1275,7 @@
       <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1272,11 +1284,11 @@
       <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="17" spans="1:8">
+    <row r="4" s="1" customFormat="1" ht="30" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1286,70 +1298,72 @@
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="17" spans="1:8">
+      <c r="H4" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="17" spans="1:8">
+      <c r="H5" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="E6" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>34</v>
+      <c r="H6" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1367,17 +1381,17 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.859375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.2890625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.2890625" style="1"/>
+    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.8571428571429" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.2857142857143" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:8">
@@ -1394,7 +1408,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
@@ -1406,7 +1420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="17" spans="1:8">
+    <row r="2" s="1" customFormat="1" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1416,11 +1430,11 @@
       <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>36</v>
+      <c r="E2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>13</v>
@@ -1428,11 +1442,11 @@
       <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="17" spans="1:8">
+    <row r="3" s="1" customFormat="1" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1442,11 +1456,11 @@
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>37</v>
+      <c r="E3" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -1454,11 +1468,11 @@
       <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="17" spans="1:8">
+    <row r="4" s="1" customFormat="1" ht="30" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1468,10 +1482,10 @@
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1480,24 +1494,24 @@
       <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="17" spans="1:8">
+      <c r="H4" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>40</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1506,24 +1520,24 @@
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" ht="17" spans="1:8">
+      <c r="H5" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>41</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1532,8 +1546,8 @@
       <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>34</v>
+      <c r="H6" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1551,16 +1565,16 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.2890625" style="1"/>
+    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5714285714286" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.2857142857143" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:7">
@@ -1577,7 +1591,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
@@ -1586,7 +1600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="2" s="1" customFormat="1" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1596,11 +1610,11 @@
       <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>43</v>
+      <c r="E2" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>13</v>
@@ -1609,7 +1623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="3" s="1" customFormat="1" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1619,11 +1633,11 @@
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>44</v>
+      <c r="E3" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>13</v>
@@ -1632,7 +1646,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="4" s="1" customFormat="1" ht="30" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1642,9 +1656,9 @@
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>45</v>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>13</v>
@@ -1653,21 +1667,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="5" s="1" customFormat="1" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>46</v>
+      <c r="D5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
@@ -1676,21 +1690,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>47</v>
+      <c r="D6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>13</v>
@@ -1710,20 +1724,20 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.2890625" style="1"/>
+    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.2857142857143" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:7">
@@ -1749,7 +1763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="2" s="1" customFormat="1" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1759,10 +1773,10 @@
       <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -1772,7 +1786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="3" s="1" customFormat="1" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1782,10 +1796,10 @@
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1795,7 +1809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="4" s="1" customFormat="1" ht="30" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1805,9 +1819,9 @@
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7" t="s">
-        <v>23</v>
+      <c r="D4" s="8"/>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>13</v>
@@ -1816,22 +1830,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="5" s="1" customFormat="1" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
@@ -1839,21 +1853,21 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="17" spans="1:7">
+    <row r="6" s="1" customFormat="1" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>13</v>
@@ -1871,23 +1885,23 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="16.8" outlineLevelRow="1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="17.2890625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.2890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1428571428571" style="1" customWidth="1"/>
     <col min="5" max="5" width="29" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.2890625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.2890625" style="1"/>
+    <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.1428571428571" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.2857142857143" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:8">
@@ -1913,15 +1927,15 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="34" spans="1:8">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>10</v>
@@ -1929,17 +1943,121 @@
       <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="30" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:8">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check in and undo check in
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/flow_definition.xlsx
+++ b/src/main/resources/input_excel_file/flow_definition.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="flow_1_player" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="57">
   <si>
     <t>flow_id</t>
   </si>
@@ -180,13 +180,28 @@
     <t>BB_VC_VST_005</t>
   </si>
   <si>
-    <t>edit_booking_1_player_id</t>
-  </si>
-  <si>
-    <t>EB_001</t>
-  </si>
-  <si>
-    <t>EB_002</t>
+    <t>check_in_bag_id</t>
+  </si>
+  <si>
+    <t>undo_check_in_bag_id</t>
+  </si>
+  <si>
+    <t>CI_001</t>
+  </si>
+  <si>
+    <t>UCI_001</t>
+  </si>
+  <si>
+    <t>CI_002</t>
+  </si>
+  <si>
+    <t>CI_003</t>
+  </si>
+  <si>
+    <t>CI_004</t>
+  </si>
+  <si>
+    <t>CI_005</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1393,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
@@ -1724,7 +1739,7 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1885,13 +1900,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="17.2857142857143" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.2857142857143" style="1" customWidth="1"/>
@@ -1900,11 +1915,12 @@
     <col min="5" max="5" width="29" style="1" customWidth="1"/>
     <col min="6" max="6" width="22.2857142857143" style="1" customWidth="1"/>
     <col min="7" max="7" width="30.5714285714286" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.1428571428571" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.2857142857143" style="1"/>
+    <col min="8" max="8" width="19.2857142857143" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.2857142857143" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:8">
+    <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1929,8 +1945,11 @@
       <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:8">
+      <c r="I1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1953,10 +1972,13 @@
         <v>14</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:8">
+        <v>51</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -1979,10 +2001,13 @@
         <v>14</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="30" spans="1:8">
+        <v>53</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="30" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -2005,10 +2030,13 @@
         <v>14</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:8">
+        <v>54</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:9">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -2031,10 +2059,13 @@
         <v>14</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:8">
+        <v>55</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
@@ -2057,7 +2088,10 @@
         <v>14</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
detail cost and detail agency paid
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/flow_definition.xlsx
+++ b/src/main/resources/input_excel_file/flow_definition.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="184">
   <si>
     <t>flow_id</t>
   </si>
@@ -494,6 +494,15 @@
     <t>e_invoice_id</t>
   </si>
   <si>
+    <t>invoice_detail_cost_id</t>
+  </si>
+  <si>
+    <t>invoice_detail_agency_paid_id</t>
+  </si>
+  <si>
+    <t>revenue_detail_report_id</t>
+  </si>
+  <si>
     <t>INPUT_PAYMENT_PLAYER1</t>
   </si>
   <si>
@@ -527,6 +536,18 @@
     <t>E_INVOICE_001</t>
   </si>
   <si>
+    <t>E_INVOICE_PLAYER1</t>
+  </si>
+  <si>
+    <t>E_INVOICE_PLAYER2</t>
+  </si>
+  <si>
+    <t>E_INVOICE_PLAYER3</t>
+  </si>
+  <si>
+    <t>E_INVOICE_PLAYER4</t>
+  </si>
+  <si>
     <t>UPDATE_AGENCY_PAY_PLAYER1_004</t>
   </si>
   <si>
@@ -542,6 +563,9 @@
     <t>E_INVOICE_002</t>
   </si>
   <si>
+    <t>E_INVOICE_AGENCY</t>
+  </si>
+  <si>
     <t>CI_EKYC_PLAYER1</t>
   </si>
   <si>
@@ -555,6 +579,9 @@
   </si>
   <si>
     <t>E_INVOICE_003</t>
+  </si>
+  <si>
+    <t>REPORT_001</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1247,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1238,9 +1265,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1984,13 +2008,13 @@
       <c r="H2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>77</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>79</v>
       </c>
       <c r="L2" s="7" t="s">
@@ -2118,13 +2142,13 @@
       <c r="H3" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>106</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="8" t="s">
         <v>108</v>
       </c>
       <c r="L3" s="7" t="s">
@@ -2250,13 +2274,13 @@
       <c r="H4" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>114</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="8" t="s">
         <v>116</v>
       </c>
       <c r="L4" s="7" t="s">
@@ -2327,13 +2351,13 @@
       <c r="H5" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>119</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="8" t="s">
         <v>121</v>
       </c>
       <c r="L5" s="7" t="s">
@@ -2404,13 +2428,13 @@
       <c r="H6" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>124</v>
       </c>
       <c r="J6" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="8" t="s">
         <v>126</v>
       </c>
       <c r="L6" s="7" t="s">
@@ -2628,10 +2652,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AK4"/>
+  <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AO15" sqref="AO15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2857142857143" defaultRowHeight="15" outlineLevelRow="3"/>
@@ -2649,10 +2673,11 @@
     <col min="20" max="22" width="18.2857142857143" style="1" customWidth="1"/>
     <col min="23" max="36" width="10.2857142857143" style="1"/>
     <col min="37" max="37" width="14.2857142857143" style="1" customWidth="1"/>
-    <col min="38" max="16384" width="10.2857142857143" style="1"/>
+    <col min="38" max="43" width="15.4285714285714" style="1" customWidth="1"/>
+    <col min="44" max="16384" width="10.2857142857143" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="60" customHeight="1" spans="1:37">
+    <row r="1" s="1" customFormat="1" ht="60" customHeight="1" spans="1:43">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2764,8 +2789,26 @@
       <c r="AK1" s="2" t="s">
         <v>153</v>
       </c>
+      <c r="AL1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="45" spans="1:37">
+    <row r="2" s="1" customFormat="1" ht="45" spans="1:43">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -2809,44 +2852,58 @@
       <c r="U2" s="7"/>
       <c r="V2" s="7"/>
       <c r="W2" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AE2" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="AF2" s="7"/>
       <c r="AG2" s="7"/>
       <c r="AH2" s="7"/>
       <c r="AI2" s="7"/>
-      <c r="AJ2" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="AK2" s="8" t="s">
-        <v>164</v>
-      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="AL2" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="AM2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="AN2" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
     </row>
-    <row r="3" s="1" customFormat="1" ht="45" spans="1:37">
+    <row r="3" s="1" customFormat="1" ht="45" spans="1:43">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -2886,16 +2943,16 @@
         <v>81</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
@@ -2906,20 +2963,28 @@
       <c r="AC3" s="7"/>
       <c r="AD3" s="7"/>
       <c r="AE3" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="AF3" s="7"/>
       <c r="AG3" s="7"/>
       <c r="AH3" s="7"/>
       <c r="AI3" s="7"/>
-      <c r="AJ3" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="AK3" s="8" t="s">
-        <v>169</v>
-      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK3" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="AL3" s="7"/>
+      <c r="AM3" s="7"/>
+      <c r="AN3" s="7"/>
+      <c r="AO3" s="7"/>
+      <c r="AP3" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AQ3" s="7"/>
     </row>
-    <row r="4" s="1" customFormat="1" ht="45" spans="1:37">
+    <row r="4" s="1" customFormat="1" ht="45" spans="1:43">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -2949,16 +3014,16 @@
         <v>26</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="Q4" s="7" t="s">
         <v>80</v>
@@ -2971,41 +3036,57 @@
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="Z4" s="7" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AA4" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="AD4" s="7" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="AE4" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="AF4" s="7"/>
       <c r="AG4" s="7"/>
       <c r="AH4" s="7"/>
       <c r="AI4" s="7"/>
-      <c r="AJ4" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="AK4" s="8" t="s">
-        <v>174</v>
+      <c r="AJ4" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK4" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL4" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="AM4" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="AN4" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="AO4" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP4" s="7"/>
+      <c r="AQ4" s="7" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>